<commit_message>
Works by Year filter
</commit_message>
<xml_diff>
--- a/Expected_demographics.xlsx
+++ b/Expected_demographics.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcarmeli/Desktop/FDA Drug Trials Snapshots/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcarmeli/Documents/GitHub/FDA_DTS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C735AF8D-D4F5-1B4F-901D-9E58D2F60046}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D03A06-E593-1A45-9338-789A380FA607}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15740" activeTab="1" xr2:uid="{B9969568-D9D4-D249-8891-44A6F8A9EC2F}"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15740" activeTab="2" xr2:uid="{B9969568-D9D4-D249-8891-44A6F8A9EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Expected_demographics" sheetId="1" r:id="rId1"/>
     <sheet name="HCV" sheetId="2" r:id="rId2"/>
+    <sheet name="Migraine" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Black</t>
   </si>
@@ -116,14 +117,51 @@
   </si>
   <si>
     <t>average</t>
+  </si>
+  <si>
+    <t>White only</t>
+  </si>
+  <si>
+    <t>Black only</t>
+  </si>
+  <si>
+    <t>American Indian or Alaska Native only</t>
+  </si>
+  <si>
+    <t>Asian only</t>
+  </si>
+  <si>
+    <t>Native Hawaiian only</t>
+  </si>
+  <si>
+    <t>2 or more races</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>% of adults with severe headache or migraine</t>
+  </si>
+  <si>
+    <t>https://www.cdc.gov/nchs/data/hus/2017/041.pdf</t>
+  </si>
+  <si>
+    <t>% of population</t>
+  </si>
+  <si>
+    <t>implied burden</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -181,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -190,6 +228,7 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +547,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -677,7 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8655B4-21C9-4344-B0FE-4ABB9BF76C0A}">
   <dimension ref="B1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -1106,4 +1145,152 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D0C076-68AA-1342-B71F-6ED9EDCC586D}">
+  <dimension ref="C1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>16</v>
+      </c>
+      <c r="E3">
+        <v>76.5</v>
+      </c>
+      <c r="F3" s="8">
+        <f>(D3/100)*E3</f>
+        <v>12.24</v>
+      </c>
+      <c r="G3" s="1">
+        <f>F3/$F$11</f>
+        <v>0.6864257073157054</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4">
+        <v>14.6</v>
+      </c>
+      <c r="E4">
+        <v>14.3</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" ref="F4:F9" si="0">(D4/100)*E4</f>
+        <v>2.0878000000000001</v>
+      </c>
+      <c r="G4" s="1">
+        <f>F4/$F$11</f>
+        <v>0.11708493396517401</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>9.9</v>
+      </c>
+      <c r="E6">
+        <v>6.8</v>
+      </c>
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.67320000000000002</v>
+      </c>
+      <c r="G6" s="1">
+        <f>F6/$F$11</f>
+        <v>3.7753413902363801E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>22.5</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9">
+        <v>15.3</v>
+      </c>
+      <c r="E9">
+        <v>18.5</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>2.8304999999999998</v>
+      </c>
+      <c r="G9" s="1">
+        <f>F9/$F$11</f>
+        <v>0.15873594481675687</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="8">
+        <f>SUM(F3:F9)</f>
+        <v>17.831499999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>